<commit_message>
dietplanner - work on xlsx data
</commit_message>
<xml_diff>
--- a/xlsxData/DaysData.xlsx
+++ b/xlsxData/DaysData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr filterPrivacy="1" hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C25445-6E8E-489F-BA10-F5B408057305}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F69524-375D-4538-AFBB-DEA082432D6D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1365" windowWidth="25440" windowHeight="15390" tabRatio="943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22380" yWindow="1560" windowWidth="18900" windowHeight="11055" tabRatio="943" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Spis" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3985" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4085" uniqueCount="336">
   <si>
     <t>Papryka czerwona</t>
   </si>
@@ -591,9 +591,6 @@
     <t>Przepis</t>
   </si>
   <si>
-    <t>Paprykę kroimy w krążki. Na klarowanym maśle podduszamy paprykę z jednej strony. Przewracamy krążek nadrugą stronę,wbijamy jajka, skręcamy ogień do minimu, przykrywamy pokrywką. Żółtko jaja ma być płynne, a białko ścięte.Gotowe jajka posypujemy szczypiorkiem</t>
-  </si>
-  <si>
     <t>Jajko sadzone w papryce</t>
   </si>
   <si>
@@ -603,33 +600,18 @@
     <t>Kasza gryczana z warzywami i pestkami dyni</t>
   </si>
   <si>
-    <t>Na oliwie podsmażamy pokrojoną w kostkę paprykę. Brokułygotujemy al dente.Ugotowaną kaszę gryczaną mieszamy z warzywami i pestkami dyni. Posypujemy dowolną zieleniną. Natką pietruszki, kolendrą,bazylią</t>
-  </si>
-  <si>
     <t>Sałatka z wyfiletowanego grejpfruta</t>
   </si>
   <si>
-    <t>Mięso oprószamy solą i pieprzem cytrynowym. Obsmażamy na klarowanym maśle po 3 minuty z każdej strony.Lekko podlewamywodą, przykrywamy pokrywką, dusimy na minimalnym ogniu przez 10 minut. Podajemy z sałatką</t>
-  </si>
-  <si>
     <t>Sałatka z filetem z indyka</t>
   </si>
   <si>
-    <t>Wszystkie składniki (oprócz owoców) zalewamy ciepłym mlekiem. Odstawiamy na 10 minut. Blendujemy zowocami</t>
-  </si>
-  <si>
     <t>Koktaj z bananem i mrożonymi owocami</t>
   </si>
   <si>
-    <t>Jabłko kroimy w drobną kostkę. Pomarańczęfiletujemy z białych błon. Kroimy w małe kawałki.</t>
-  </si>
-  <si>
     <t>Makaron z sosem pomidorowym</t>
   </si>
   <si>
-    <t>Cebulę kroimy w kosteczkę, rumienimy na klarowanymmaśle. Dodajemy pomidory, smażymy aż o połowę zderukuje się ilośćwody. Doprawiamy do smaku solą, słodką papryką, szczyptą ksylitolu i pieprzu. Mieszamy z poszarpanymilistkami bazylii.Mieszamy z ugotowanym ale dente makaronem. Posypujemy migdałami.</t>
-  </si>
-  <si>
     <t>Sałatka z pamidorami i oliwkami</t>
   </si>
   <si>
@@ -642,12 +624,6 @@
     <t>Kanapka z szynką i serkiem arla</t>
   </si>
   <si>
-    <t>Pomarańczę filetujemy (usuwamy białe błony). Kroimyw kawałki. Mieszamy z pokrojonym w kosteczkę jabłkiem i dodatkami</t>
-  </si>
-  <si>
-    <t>Na dnie naczynia żaroodpornego układamy szpinak. Kładziemy dorsza oprószonego solą i pieprzem cytrynowym. Na klarowanymmaśle szklimy pokrojoną w półtalarki białą część pora. Wylewamy na rybę. Przykrywamy pokrywę naczyniażaroodpornego.Zapiekamy w piekarniku nagrzanym do 200 stopni przez 15 minut. Podajemy z marchewką gotowaną na parze!! Skropioną oliwą.</t>
-  </si>
-  <si>
     <t>Dorsz pieczony z marchewką, szpinakiem i porem</t>
   </si>
   <si>
@@ -657,15 +633,9 @@
     <t>Zupa krem z zielonego groszku</t>
   </si>
   <si>
-    <t>Na klarowanym maślepodduszamy warzywa. Zalewamy bulionem, gotujemy domiękkości.Blendujemy na krem.</t>
-  </si>
-  <si>
     <t>Koktajl na ciepło z jabłkiem</t>
   </si>
   <si>
-    <t>Płatki i nasiona chia zalewamy ciepłym mlekiem. Odstawiamy na 10 minut. Jabłko ścieramy na grubej tarce. Mieszamy zcynamonem, rozgnienionymi orzechami i mlekiem z płatkami.</t>
-  </si>
-  <si>
     <t>Sałatka z kaszą, rzodkiewką i ogórkiem</t>
   </si>
   <si>
@@ -675,9 +645,6 @@
     <t>Wegetariańska faszerowana papryka</t>
   </si>
   <si>
-    <t>Ryż szklimy na oleju. Zalewamy wodą. Gotujemy do miękkości. Startąna tarce marchewmieszamy z curry i imbirem. Dodajemy do ryżu razemz posiekaną natką pietruszki.Papryki podpiekamy przez 15 minut w temperaturze 200 stopni. Wyjmujemy, wypełniamy farszem i ponowniezapiekamy przez 15minut</t>
-  </si>
-  <si>
     <t>Jabłko z migdałami</t>
   </si>
   <si>
@@ -693,18 +660,12 @@
     <t>Sałatka owocowa z grejpfrutem i gruszką</t>
   </si>
   <si>
-    <t>Rybę opruszamy solą i pieprzem cytrynowym. Pieczemy25 minut w 200 stopniach.Warzywa gotowane na parze, skropione oliwą. Posypane rozgniecionymi pestkami dyni.</t>
-  </si>
-  <si>
     <t>Łosoś pieczony z brokułem i marchwią</t>
   </si>
   <si>
     <t>Kanapka z pastą roślinną</t>
   </si>
   <si>
-    <t>Na maśle podduszmay białą część pora. Dodajemy pozostałe warzywa. Zalewamy 300 ml wody. Gotujemy do miękkości zdodatkiem listka laurowego, soli, pieprzu i ziela angielskiego. Wymujemy listek i ziele. Blendujemy zupę. Na wierzch dodajemyoliwę. Jeśli zupa jest zbyt łagodna, dopraw mocniejnp. curry lub imbirem</t>
-  </si>
-  <si>
     <t>Zupa warzywna z selerem, porem, pietruszką, ziemniakami i brokułami</t>
   </si>
   <si>
@@ -732,30 +693,18 @@
     <t>Pieczone udko z mizerią</t>
   </si>
   <si>
-    <t>Pieczone udko. Mizeria. Ziemniaki pokrojone w talarki. Ugotowane na parze</t>
-  </si>
-  <si>
     <t>Sałatka z kaszą, cukinią i rzodkiewką</t>
   </si>
   <si>
-    <t>Pokrojoną w kosteczkę cukinię podduszamy na klarowanym maśle. Ma być al dente. Mieszamyz ugotowaną kaszą. Pokrrojoną wkosteczkę rzodkiewką, ziarnami i sosem</t>
-  </si>
-  <si>
     <t>Omlet ze szpinakiem i porem</t>
   </si>
   <si>
-    <t>Na klarowamy maśle szklimy białą część porapokrojoną w półtalarki. Dodajemy poszarpany szpinak wymieszany zroztrzepanymi jajkami. Doprawiamy świeżo zmielonympieprzem. Wylewamy na patelnię</t>
-  </si>
-  <si>
     <t>Kanapka z pesto, szynką i ogórkiem</t>
   </si>
   <si>
     <t>Sałatka owocowa z jabłkiem i kiwi</t>
   </si>
   <si>
-    <t>Paprykę kroimy w paseczki, cukinię w półtalarki. Szklimy na klarowanym maśle razem z pokrojonym w kosteczkę mięsem .Zalewamy mlekiem kokosowym wymieszanym z curry i pieprzem cytrynowym. Na dnie naczynia do zapiekania układamy szpinak,na nim warzywa z mlekiem kokosowym. Całość posypujemy fetą. Pieczemy 15 minut w 200 stopniach</t>
-  </si>
-  <si>
     <t>Filet z kurczaka zapiekany z cukinią, szpinakiem i serem feta</t>
   </si>
   <si>
@@ -765,7 +714,325 @@
     <t>Zupa krem z selera i pietruszki</t>
   </si>
   <si>
-    <t>Warzywa zalewamy bulionem warzywnym. Gotujemy do miękkości, blendujemy, solimy (w zależnościod tego jak doprawiony jest bulion).Zupę już na talerzu mieszamy z oliwą. Polecam doprawić białym pieprzem i curry</t>
+    <t>Placuszki bananowe owsiane</t>
+  </si>
+  <si>
+    <t>Sałatka z ogórkiem, rzodkiewką, serem feta i makaronem</t>
+  </si>
+  <si>
+    <t>Mintaj pieczony w sosie pomidorowym</t>
+  </si>
+  <si>
+    <t>Pomelo z sezamem</t>
+  </si>
+  <si>
+    <t>Cukinia zapiekana z papryką i cebulą</t>
+  </si>
+  <si>
+    <t>Jajecznica ze szczypiorkiem</t>
+  </si>
+  <si>
+    <t>Jajecznica ze szczypiorkiem. Polędwicę jemy osobno.</t>
+  </si>
+  <si>
+    <t>Sałatka z pomelo, kiwi i nasionami chia</t>
+  </si>
+  <si>
+    <t>Kurczak marynowany w pesto</t>
+  </si>
+  <si>
+    <t>Jogurt z granolą</t>
+  </si>
+  <si>
+    <t>Warzywa na patelni</t>
+  </si>
+  <si>
+    <t>Pieczone udko. Mizeria. Ziemniaki pokrojone w talarki. Ugotowane na parze.</t>
+  </si>
+  <si>
+    <t>Koktjl śniadaniowy z bananem i płatkami owsianymi</t>
+  </si>
+  <si>
+    <t>Sałatka z makaronem, brokułami, papryką i fasolką szparagową</t>
+  </si>
+  <si>
+    <t>Brokuły ugotowane. Papryka pokrojona w kosteczkę, podduszona na klarowanym maśle.</t>
+  </si>
+  <si>
+    <t>Makaron w sosie pomidorowym z serem feta</t>
+  </si>
+  <si>
+    <t>Kanapka z pesto i wędliną</t>
+  </si>
+  <si>
+    <t>Sałatka z cieciorką, rzodkiewką, ogórkiem i sałatą</t>
+  </si>
+  <si>
+    <t>Omlet z wędzonym łososiem, sezamem i szczypiorkiem</t>
+  </si>
+  <si>
+    <t>Kanapka z ogórkiem, wędliną + sok warzywny</t>
+  </si>
+  <si>
+    <t>Pieczone warzywa, cukinia, marchew, bataty</t>
+  </si>
+  <si>
+    <t>Grejpfrut z sezamem</t>
+  </si>
+  <si>
+    <t>Sałatka z papryką, cieciorką i sałatą</t>
+  </si>
+  <si>
+    <t>Kanapka z łososiem, sałatą i pomidorem</t>
+  </si>
+  <si>
+    <t>Koktajl z czerwonymi owocami i bananem</t>
+  </si>
+  <si>
+    <t>Indyk w jarzynach</t>
+  </si>
+  <si>
+    <t>Cukinia faszerowana marchewką, fetą i pomidorami</t>
+  </si>
+  <si>
+    <t>Koktajl szarlotkowy</t>
+  </si>
+  <si>
+    <t>Grejpfrut z orzechami</t>
+  </si>
+  <si>
+    <t>Jogurt z dżemem i nasionami chia</t>
+  </si>
+  <si>
+    <t>Sałatka z pomidorami koktajlowymi, papryką i sałatą</t>
+  </si>
+  <si>
+    <t>Twarożek ze szczypiorkiem i papryką</t>
+  </si>
+  <si>
+    <t>Pudding owocowy z chia</t>
+  </si>
+  <si>
+    <t>Dorsz pieczony z kaszą i groszkiem</t>
+  </si>
+  <si>
+    <t>Sałatka makaronowa z szynką</t>
+  </si>
+  <si>
+    <t>Ugotowany al dente makaron mieszamy z pokrojoną w paseczki szynką i oliwkami. Dodajemyfasolkę szparagową, skrapiamy oliwą.</t>
+  </si>
+  <si>
+    <t>Warzywa podduszamy na klarowanym maśle. Zalewamy wywarem, gotujemy do miekkości. Blendujemy na gładką masę. Polecam doprawić białym pieprzem. Na wierzch zupy dodajemy zimną oliwę.</t>
+  </si>
+  <si>
+    <t>Fileta z dorsza oprószamy solą i pieprzem cytrynowym. Skrapiamy oliwą, posypujemy koperkiem, i pieczemy 10-15 minut w temperaturze 180 st. Polecam zawinąć w pergamin aby ryba była soczysta.Kaszę szklimy na klarowanym maśle, dodajemy groszek, zalewamy wodą, gotujemy do miękkości. Kaszę gotujemy z łyżeczką oliwy.</t>
+  </si>
+  <si>
+    <t>Jabłko kroimy w kosteczkę. Wkładamy do garnka, delikatnie podlewamy wodą i lekko dodduszamy. Mieszamy ze startą na tarce surową gruszką, otrębami, orzechami, nasionami chia (napęcznieją pod wpływem płynu) oraz cynamonem. Odsatwiamy.</t>
+  </si>
+  <si>
+    <t>Twarożek ucieramy z jogurtem. Dodajemy drobniutko posiekaną paprykę i szczypiorek. Doprawiamy do smaku solą i pieprzem.</t>
+  </si>
+  <si>
+    <t>Odstawiamy na 10 minut aby nasionka napęczniały. Na dnie kubka kładziemy konfiturę z jagód (można użyć innej).  Zalewamy jogurtem.</t>
+  </si>
+  <si>
+    <t>Indyka solimy i oprószamy curry. Obtaczamy w mące kukurydzianej, smażymy na klarowanym maśle. Usmażone mięso zakrywamy startymi na grubej tarce warzywami i podlewamy bulionem wrzywnym. Dusimy 30 minut. Wyjmujemy mięso, wrzywa z bulionem blebdujemy na sos. Dodajemy koperek.</t>
+  </si>
+  <si>
+    <t>Cukinię przekrawamy na pół. Wkładamy do piekarnika nagrzanego do 200stopni na 15 minut. Z cukinii wydrążamy środek. Kroimy w kosteczkę, mieszamy ze startą na drobniutkiej tarce marchewką, pokruszoną fetą i pokrojonymi drobniutko suszonymi pomidorami. Napełniamy farszem łódeczki. Wkładamy do piekarnika na 15minut.</t>
+  </si>
+  <si>
+    <t>Marchew i pietruszkę ścieramy na tarce. Cukinię kroimy w połtaraki. Warzywa podduszamy lekko na klarowanym maśle. Doprawiamy curry i słodką papryką. Na dnie naczynia żaroodpornego układamy pokrojone w talarki bataty. Przykrywamy warzywami. Pieczemy 30 munut w 200 stopniach.</t>
+  </si>
+  <si>
+    <t>Na oliwie podsmażamy pomidorki, aż odparuje woda. Dodajemy bazylię, mieszamy z makaronem i fetą.</t>
+  </si>
+  <si>
+    <t>Warzywa tzw. na patelnię (polecam Frosta warzywa w kolorze zielonym, żółtym i czerownym do wyboru -bez ziemniaków). Rozmrażamy warzywa, podsmażamy na oleju. Można użyć dowolnych świeżych warzyw zachowując gramaturę.</t>
+  </si>
+  <si>
+    <t>Mięso nacieramy solą i pesto, zawijamy w pergamin, smażymy na suchej patelni po 2 minuty z każdej strony. Ryż gotujemy do miękkości. Na rozgrzany olej wrzucamy curry, po chwili dodajemy ryż i dowolną zieleninę.</t>
+  </si>
+  <si>
+    <t>Cukinię przekrawamy na pół. Wkładamy do piekarnika nagrzanego do 200 stopni na 15 minut. Po tym czasie przy pomocy łyżeczki wydrążamy środek. Na klarowanym maśle podduszamy pokrojoną w kosteczkę cebulę. Do zrumienionej dodajemy pokrojoną w kosteczkę paprykę i smażymy aż połowa wody z papryki odparuje. Składniki z patelni mieszamy z posiekanym drobno wydrążonym środkiem z cukinii dodając pieprz i curry. Powstałym farszem wypełniamy cukinie i ponownie wstawiamy do piekarnika na 20minut.</t>
+  </si>
+  <si>
+    <t>Na klarowanym maśle szklimy starte na tarce warzywa. Zalewamy pomidorami. Dodajemy curry, słodką paprykę,sól i koperek. Redukujemy płyn do połowy. Rybę oprószamy solą i curry. Zalewamy sosem. Zapiekamy 15 minut w 200 stopniach.</t>
+  </si>
+  <si>
+    <t>Banana miksujemy z jajkiem. Mieszamy z mąką owsianą. Odstawiamy na 2-3 minuty. Smażymy na klarowanym maśle lub oleju.</t>
+  </si>
+  <si>
+    <t>Warzywa zalewamy bulionem warzywnym. Gotujemy do miękkości, blendujemy, solimy (w zależnościod tego jak doprawiony jest bulion). Zupę już na talerzu mieszamy z oliwą. Polecam doprawić białym pieprzem i curry.</t>
+  </si>
+  <si>
+    <t>Paprykę kroimy w paseczki, cukinię w półtalarki. Szklimy na klarowanym maśle razem z pokrojonym w kosteczkę mięsem. Zalewamy mlekiem kokosowym wymieszanym z curry i pieprzem cytrynowym. Na dnie naczynia do zapiekania układamy szpinak,na nim warzywa z mlekiem kokosowym. Całość posypujemy fetą. Pieczemy 15 minut w 200 stopniach.</t>
+  </si>
+  <si>
+    <t>Na klarowamy maśle szklimy białą część pora pokrojoną w półtalarki. Dodajemy poszarpany szpinak wymieszany z roztrzepanymi jajkami. Doprawiamy świeżo zmielonym pieprzem. Wylewamy na patelnię.</t>
+  </si>
+  <si>
+    <t>Pokrojoną w kosteczkę cukinię podduszamy na klarowanym maśle. Ma być al dente. Mieszamy z ugotowaną kaszą. Pokrojoną w kosteczkę rzodkiewką, ziarnami i sosem.</t>
+  </si>
+  <si>
+    <t>Na maśle podduszmay białą część pora. Dodajemy pozostałe warzywa. Zalewamy 300 ml wody. Gotujemy do miękkości z dodatkiem listka laurowego, soli, pieprzu i ziela angielskiego. Wymujemy listek i ziele. Blendujemy zupę. Na wierzch dodajemy oliwę. Jeśli zupa jest zbyt łagodna, dopraw mocniej np. curry lub imbirem.</t>
+  </si>
+  <si>
+    <t>Rybę opruszamy solą i pieprzem cytrynowym. Pieczemy 25 minut w 200 stopniach. Warzywa gotowane na parze, skropione oliwą. Posypane rozgniecionymi pestkami dyni.</t>
+  </si>
+  <si>
+    <t>Ryż szklimy na oleju. Zalewamy wodą. Gotujemy do miękkości. Startą na tarce marchew mieszamy z curry i imbirem. Dodajemy do ryżu razem z posiekaną natką pietruszki. Papryki podpiekamy przez 15 minut w temperaturze 200 stopni. Wyjmujemy, wypełniamy farszem i ponownie zapiekamy przez 15 minut.</t>
+  </si>
+  <si>
+    <t>Płatki i nasiona chia zalewamy ciepłym mlekiem. Odstawiamy na 10 minut. Jabłko ścieramy na grubej tarce. Mieszamy z cynamonem, rozgnienionymi orzechami i mlekiem z płatkami.</t>
+  </si>
+  <si>
+    <t>Na klarowanym maśle podduszamy warzywa. Zalewamy bulionem, gotujemy do miękkości. Blendujemy na krem.</t>
+  </si>
+  <si>
+    <t>Na dnie naczynia żaroodpornego układamy szpinak. Kładziemy dorsza oprószonego solą i pieprzem cytrynowym. Na klarowanym maśle szklimy pokrojoną w półtalarki białą część pora. Wylewamy na rybę. Przykrywamy pokrywę naczyniaża roodpornego. Zapiekamy w piekarniku nagrzanym do 200 stopni przez 15 minut. Podajemy z marchewką gotowaną na parze!!  Skropioną oliwą.</t>
+  </si>
+  <si>
+    <t>Pomarańczę filetujemy (usuwamy białe błony). Kroimy w kawałki. Mieszamy z pokrojonym w kosteczkę jabłkiem i dodatkami.</t>
+  </si>
+  <si>
+    <t>Cebulę kroimy w kosteczkę, rumienimy na klarowanym maśle. Dodajemy pomidory, smażymy aż o połowę zderukuje się ilość wody. Doprawiamy do smaku solą, słodką papryką, szczyptą ksylitolu i pieprzu. Mieszamy z poszarpanymi listkami bazylii. Mieszamy z ugotowanym ale dente makaronem. Posypujemy migdałami.</t>
+  </si>
+  <si>
+    <t>Jabłko kroimy w drobną kostkę. Pomarańczę filetujemy z białych błon. Kroimy w małe kawałki.</t>
+  </si>
+  <si>
+    <t>Wszystkie składniki (oprócz owoców) zalewamy ciepłym mlekiem. Odstawiamy na 10 minut. Blendujemy z owocami.</t>
+  </si>
+  <si>
+    <t>Mięso oprószamy solą i pieprzem cytrynowym. Obsmażamy na klarowanym maśle po 3 minuty z każdej strony. Lekko podlewamy wodą, przykrywamy pokrywką, dusimy na minimalnym ogniu przez 10 minut. Podajemy z sałatką.</t>
+  </si>
+  <si>
+    <t>Na oliwie podsmażamy pokrojoną w kostkę paprykę. Brokuły gotujemy al dente. Ugotowaną kaszę gryczaną mieszamy z warzywami i pestkami dyni. Posypujemy dowolną zieleniną. Natką pietruszki, kolendrą, bazylią.</t>
+  </si>
+  <si>
+    <t>Paprykę kroimy w krążki. Na klarowanym maśle podduszamy paprykę z jednej strony. Przewracamy krążek nadrugą stronę, wbijamy jajka, skręcamy ogień do minimum, przykrywamy pokrywką. Żółtko jaja ma być płynne, a białko ścięte. Gotowe jajka posypujemy szczypiorkiem.</t>
+  </si>
+  <si>
+    <t>Zupza z zemniakiem, pietruszką i brokułami</t>
+  </si>
+  <si>
+    <t>Sałatka z gruszką, orzechami i papryką</t>
+  </si>
+  <si>
+    <t>Cieciorka z cukinią i ryżem w mleku kokosowym</t>
+  </si>
+  <si>
+    <t>Na patelnię wlewamy mleko kokosowe. Dodajemy cieciorkę z puszki, łyżeczkę curry, szczyptę imbiru i świeżą kolendę. Jak się zagotuje dodajemy pokrojoną w półtalarki cukinię. Gotujemy 2 minuty. Jemy z ryżem.</t>
+  </si>
+  <si>
+    <t>Kanapka z hummusem i sałatą</t>
+  </si>
+  <si>
+    <t>Sałatka z brokułem i serem feta</t>
+  </si>
+  <si>
+    <t>Ugotowane różyczki brokuła mieszamy z pestkami dyni i oliwą.</t>
+  </si>
+  <si>
+    <t>Koktajl śniadaniowy z czerwonymi owocami, i bananem</t>
+  </si>
+  <si>
+    <t>Sałatka owocowa z pomarańczą i gruszką</t>
+  </si>
+  <si>
+    <t>Kurczak w sosie z pieczarkami</t>
+  </si>
+  <si>
+    <t>Fileta z kurczaka nacieramy czosnkiem, kurkumą, szczyptą curry i solą. Odstawiamy na kilkanaście minut (może być na dłużej). Na klarowanym maśle obsmażamy fileta z obydwu stron. Zdejmujemy z patelni. Odstawiamy na bok. Na patelnię wrzucamy pokrojone w kawałki pieczarki, soliny, obsmażamy, zdejmujemy z patelni. Mąkę mieszamy z mlekiem, wylewamy na patelnię (wysoką), mieszamy aż lekko zgęstnieje. Do mleka wkładamy kurczaka i pieczarki. Dusimy 20 minut na małym ogniu. Doprawiamy koperkiem.</t>
+  </si>
+  <si>
+    <t>Tzatziki</t>
+  </si>
+  <si>
+    <t>Warzywa ścieramy na grubej tarce. Mieszamy z jogurtem, dprawiamy do smaku.</t>
+  </si>
+  <si>
+    <t>Podsmażane warzywa</t>
+  </si>
+  <si>
+    <t>Rozmrażamy warzywa, podsmażamy na oleju. Można użyć dowolnych świeżych warzyw zachowując gramaturę.</t>
+  </si>
+  <si>
+    <t>Kanapka z wędliną, pomidorem sałatą i pesto</t>
+  </si>
+  <si>
+    <t>Sałatka z makaronem, papryką, pomidorem</t>
+  </si>
+  <si>
+    <t>Sałatka owocowa z jabłkiem</t>
+  </si>
+  <si>
+    <t>Sałatka z cukinii, cieciorki i sałaty</t>
+  </si>
+  <si>
+    <t>Cukinia pokrojona w talarki. Podgrillowana na suchej patelni.</t>
+  </si>
+  <si>
+    <t>Placuszki bananowe na jogurcie</t>
+  </si>
+  <si>
+    <t>Banana miksujemy z jajkiem i jogurtem. Mieszamy z płatkami. Odstawiamy na 5 minut. Smażymy.</t>
+  </si>
+  <si>
+    <t>Surówka z jabłka i marchwi</t>
+  </si>
+  <si>
+    <t>Marchew i jabłko ścieramy na grubej tarce.</t>
+  </si>
+  <si>
+    <t>Sałatka z kaszy z dodatkami</t>
+  </si>
+  <si>
+    <t>Na oliwie szklimy kaszę. Zalewamy bulionem warzywnym. Goujemy do miękkości. Na klarowanym maśle podsmażamy cukinię pokrojoną w kosteczkę. Mieszamy z ugotowaną kaszą, dodatkami i dowolną zieleniną.</t>
+  </si>
+  <si>
+    <t>Jogurt mieszamy z chia i płaską łyżką ksylitolu. Odstawiamy na 5 minut.Na dnie naczynia kładziemy konfiturę, zalewamy jogurtem.</t>
+  </si>
+  <si>
+    <t>Pieczony dorsz podawany z ogórkiem</t>
+  </si>
+  <si>
+    <t>Rybę oprószamy curry i pieprzem cytrynowym. Zawijamy w papier do pieczenia, pieczemy 15 minut w 200 stopniach. Ogórka kroimy w talarki.</t>
+  </si>
+  <si>
+    <t>Koktajl śniadaniowy z czerwonymi owocami i bananem</t>
+  </si>
+  <si>
+    <t>Pieczone udko z ziemniakami, fasolką i marchwią</t>
+  </si>
+  <si>
+    <t>Udko oprószamy solą i majerankiem. Zawijamy w rękaw do pieczenia, podlewamy delikatnie wodą. Pieczemy w piekarniku. Marchew i ziemniaka kroimy w talatki. Gotujemy na parze. Skrapiamy oliwą z oliwek.</t>
+  </si>
+  <si>
+    <t>Koktajl z kiwi i bananem</t>
+  </si>
+  <si>
+    <t>Sałatka z grilowaną papryką i sałatą</t>
+  </si>
+  <si>
+    <t>Łosoś pieczony z papryką i cukinią</t>
+  </si>
+  <si>
+    <t>Do naczynia żaroodpornego wkładamy łososia. Oprószamy solą i pieprzem cytrynowym. Przykrywamy warzywami wymieszanymi z ziołamiprowansalskimi, skrapiamy oliwą. Pieczemy 30 minut w temperaturze 200 stopni.</t>
+  </si>
+  <si>
+    <t>Dowolna słodkość</t>
+  </si>
+  <si>
+    <t>Sałatka z cieciorką, serem feta i pomidorem</t>
+  </si>
+  <si>
+    <t>Placek owsiany</t>
+  </si>
+  <si>
+    <t>Żółtka oddzielamy od białka. Białko ubijamy na sztywną pianę, żółtka przekładamy do miski i mieszamy z płatami owsianymi, cynamonem, otrębami i startym na tarce jabłkiem. Następnie delikatnie łączymy z pianą z białek. Smażymy na rozgrzanej patelni na złoty kolor.</t>
   </si>
 </sst>
 </file>
@@ -781,12 +1048,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -801,9 +1074,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1088,15 +1364,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1307"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="D186" sqref="D186"/>
+    <sheetView tabSelected="1" topLeftCell="A492" workbookViewId="0">
+      <selection activeCell="C509" sqref="C509"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" style="1" customWidth="1"/>
     <col min="5" max="5" width="40.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1131,10 +1407,10 @@
         <v>62</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>295</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>0</v>
@@ -1232,7 +1508,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>6</v>
@@ -1305,10 +1581,10 @@
         <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>192</v>
+        <v>294</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>11</v>
@@ -1381,7 +1657,7 @@
         <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>15</v>
@@ -1426,10 +1702,10 @@
         <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>194</v>
+        <v>293</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>17</v>
@@ -1527,10 +1803,10 @@
         <v>62</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>196</v>
+        <v>292</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>16</v>
@@ -1603,10 +1879,10 @@
         <v>63</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>198</v>
+        <v>291</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>23</v>
@@ -1665,10 +1941,10 @@
         <v>64</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D38" t="s">
-        <v>200</v>
+        <v>290</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>25</v>
@@ -1766,7 +2042,7 @@
         <v>65</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>4</v>
@@ -1825,7 +2101,7 @@
         <v>66</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="E49" s="1" t="s">
         <v>18</v>
@@ -1898,7 +2174,7 @@
         <v>62</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>4</v>
@@ -1957,10 +2233,10 @@
         <v>63</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="D58" t="s">
-        <v>205</v>
+        <v>289</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>24</v>
@@ -2019,10 +2295,10 @@
         <v>64</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="D62" t="s">
-        <v>206</v>
+        <v>288</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>34</v>
@@ -2109,10 +2385,10 @@
         <v>65</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="D68" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>11</v>
@@ -2185,10 +2461,10 @@
         <v>66</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>210</v>
+        <v>287</v>
       </c>
       <c r="E73" s="1" t="s">
         <v>40</v>
@@ -2261,10 +2537,10 @@
         <v>62</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>212</v>
+        <v>286</v>
       </c>
       <c r="E78" s="1" t="s">
         <v>21</v>
@@ -2348,7 +2624,7 @@
         <v>63</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="E84" s="1" t="s">
         <v>9</v>
@@ -2435,10 +2711,10 @@
         <v>64</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>216</v>
+        <v>285</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>0</v>
@@ -2533,7 +2809,7 @@
         <v>65</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>23</v>
@@ -2564,7 +2840,7 @@
         <v>66</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="E99" s="1" t="s">
         <v>18</v>
@@ -2637,10 +2913,10 @@
         <v>62</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="E104" s="1" t="s">
         <v>48</v>
@@ -2713,7 +2989,7 @@
         <v>63</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="E109" s="1" t="s">
         <v>15</v>
@@ -2772,10 +3048,10 @@
         <v>64</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>222</v>
+        <v>284</v>
       </c>
       <c r="E113" s="1" t="s">
         <v>51</v>
@@ -2848,7 +3124,7 @@
         <v>65</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="E118" s="1" t="s">
         <v>4</v>
@@ -2921,10 +3197,10 @@
         <v>66</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>225</v>
+        <v>283</v>
       </c>
       <c r="E123" s="1" t="s">
         <v>3</v>
@@ -3047,10 +3323,10 @@
         <v>62</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>228</v>
+        <v>215</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="E132" s="1" t="s">
         <v>21</v>
@@ -3137,7 +3413,7 @@
         <v>63</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="E138" s="1" t="s">
         <v>50</v>
@@ -3196,7 +3472,7 @@
         <v>64</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="E142" s="1" t="s">
         <v>56</v>
@@ -3269,7 +3545,7 @@
         <v>65</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
       <c r="E147" s="1" t="s">
         <v>4</v>
@@ -3328,7 +3604,7 @@
         <v>66</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="E151" s="1" t="s">
         <v>58</v>
@@ -3401,7 +3677,7 @@
         <v>62</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>233</v>
+        <v>220</v>
       </c>
       <c r="E156" s="1" t="s">
         <v>56</v>
@@ -3499,10 +3775,10 @@
         <v>64</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>234</v>
+        <v>221</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="E163" s="1" t="s">
         <v>60</v>
@@ -3561,10 +3837,10 @@
         <v>65</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>237</v>
+        <v>282</v>
       </c>
       <c r="E167" s="1" t="s">
         <v>11</v>
@@ -3651,10 +3927,10 @@
         <v>66</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c r="E173" s="1" t="s">
         <v>1</v>
@@ -3713,7 +3989,7 @@
         <v>62</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>4</v>
@@ -3772,7 +4048,7 @@
         <v>63</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>23</v>
@@ -3831,10 +4107,10 @@
         <v>64</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>242</v>
+        <v>280</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>44</v>
@@ -3957,7 +4233,7 @@
         <v>65</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>11</v>
@@ -4030,10 +4306,10 @@
         <v>66</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>42</v>
@@ -4091,6 +4367,12 @@
       <c r="B203" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C203" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D203" s="1" t="s">
+        <v>278</v>
+      </c>
       <c r="E203" s="1" t="s">
         <v>22</v>
       </c>
@@ -4161,6 +4443,9 @@
       <c r="B208" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C208" s="1" t="s">
+        <v>230</v>
+      </c>
       <c r="E208" s="1" t="s">
         <v>39</v>
       </c>
@@ -4245,6 +4530,12 @@
       <c r="B214" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C214" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D214" s="1" t="s">
+        <v>277</v>
+      </c>
       <c r="E214" s="1" t="s">
         <v>88</v>
       </c>
@@ -4340,6 +4631,9 @@
       <c r="B221" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C221" s="1" t="s">
+        <v>232</v>
+      </c>
       <c r="E221" s="1" t="s">
         <v>89</v>
       </c>
@@ -4368,6 +4662,12 @@
       <c r="B223" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C223" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D223" t="s">
+        <v>276</v>
+      </c>
       <c r="E223" s="1" t="s">
         <v>44</v>
       </c>
@@ -4424,6 +4724,12 @@
       <c r="B227" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C227" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D227" s="1" t="s">
+        <v>235</v>
+      </c>
       <c r="E227" s="1" t="s">
         <v>1</v>
       </c>
@@ -4494,6 +4800,9 @@
       <c r="B232" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C232" s="1" t="s">
+        <v>236</v>
+      </c>
       <c r="E232" s="1" t="s">
         <v>89</v>
       </c>
@@ -4550,6 +4859,12 @@
       <c r="B236" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C236" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D236" t="s">
+        <v>275</v>
+      </c>
       <c r="E236" s="1" t="s">
         <v>46</v>
       </c>
@@ -4620,6 +4935,9 @@
       <c r="B241" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C241" s="1" t="s">
+        <v>238</v>
+      </c>
       <c r="E241" s="1" t="s">
         <v>49</v>
       </c>
@@ -4648,6 +4966,12 @@
       <c r="B243" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C243" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D243" s="1" t="s">
+        <v>274</v>
+      </c>
       <c r="E243" s="1" t="s">
         <v>92</v>
       </c>
@@ -4690,6 +5014,9 @@
       <c r="B246" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C246" s="1" t="s">
+        <v>241</v>
+      </c>
       <c r="E246" s="1" t="s">
         <v>93</v>
       </c>
@@ -4774,6 +5101,12 @@
       <c r="B252" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C252" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D252" s="1" t="s">
+        <v>243</v>
+      </c>
       <c r="E252" s="1" t="s">
         <v>12</v>
       </c>
@@ -4872,6 +5205,12 @@
       <c r="B259" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C259" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D259" s="1" t="s">
+        <v>273</v>
+      </c>
       <c r="E259" s="1" t="s">
         <v>26</v>
       </c>
@@ -4956,6 +5295,9 @@
       <c r="B265" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C265" s="1" t="s">
+        <v>245</v>
+      </c>
       <c r="E265" s="1" t="s">
         <v>4</v>
       </c>
@@ -4998,6 +5340,9 @@
       <c r="B268" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C268" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="E268" s="1" t="s">
         <v>18</v>
       </c>
@@ -5082,6 +5427,9 @@
       <c r="B274" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C274" s="1" t="s">
+        <v>247</v>
+      </c>
       <c r="E274" s="1" t="s">
         <v>1</v>
       </c>
@@ -5166,6 +5514,9 @@
       <c r="B280" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C280" s="1" t="s">
+        <v>248</v>
+      </c>
       <c r="E280" s="1" t="s">
         <v>4</v>
       </c>
@@ -5222,6 +5573,12 @@
       <c r="B284" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C284" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="D284" s="1" t="s">
+        <v>272</v>
+      </c>
       <c r="E284" s="1" t="s">
         <v>44</v>
       </c>
@@ -5292,6 +5649,9 @@
       <c r="B289" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C289" s="1" t="s">
+        <v>250</v>
+      </c>
       <c r="E289" s="1" t="s">
         <v>15</v>
       </c>
@@ -5320,6 +5680,9 @@
       <c r="B291" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C291" s="1" t="s">
+        <v>251</v>
+      </c>
       <c r="E291" s="1" t="s">
         <v>58</v>
       </c>
@@ -5390,6 +5753,9 @@
       <c r="B296" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C296" s="1" t="s">
+        <v>252</v>
+      </c>
       <c r="E296" s="1" t="s">
         <v>95</v>
       </c>
@@ -5460,6 +5826,9 @@
       <c r="B301" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C301" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="E301" s="1" t="s">
         <v>21</v>
       </c>
@@ -5516,6 +5885,12 @@
       <c r="B305" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C305" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D305" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="E305" s="1" t="s">
         <v>17</v>
       </c>
@@ -5628,6 +6003,9 @@
       <c r="B313" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C313" s="1" t="s">
+        <v>253</v>
+      </c>
       <c r="E313" s="1" t="s">
         <v>21</v>
       </c>
@@ -5684,6 +6062,12 @@
       <c r="B317" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C317" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D317" s="1" t="s">
+        <v>271</v>
+      </c>
       <c r="E317" s="1" t="s">
         <v>44</v>
       </c>
@@ -5740,6 +6124,9 @@
       <c r="B321" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C321" s="1" t="s">
+        <v>256</v>
+      </c>
       <c r="E321" s="1" t="s">
         <v>93</v>
       </c>
@@ -5796,6 +6183,9 @@
       <c r="B325" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C325" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="E325" s="1" t="s">
         <v>15</v>
       </c>
@@ -5824,6 +6214,12 @@
       <c r="B327" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C327" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="D327" s="1" t="s">
+        <v>270</v>
+      </c>
       <c r="E327" s="1" t="s">
         <v>17</v>
       </c>
@@ -5922,6 +6318,12 @@
       <c r="B334" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C334" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D334" s="1" t="s">
+        <v>269</v>
+      </c>
       <c r="E334" s="1" t="s">
         <v>49</v>
       </c>
@@ -5964,6 +6366,9 @@
       <c r="B337" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C337" s="1" t="s">
+        <v>259</v>
+      </c>
       <c r="E337" s="1" t="s">
         <v>58</v>
       </c>
@@ -6034,6 +6439,12 @@
       <c r="B342" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C342" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D342" s="1" t="s">
+        <v>268</v>
+      </c>
       <c r="E342" s="1" t="s">
         <v>48</v>
       </c>
@@ -6090,6 +6501,12 @@
       <c r="B346" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C346" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D346" s="1" t="s">
+        <v>267</v>
+      </c>
       <c r="E346" s="1" t="s">
         <v>23</v>
       </c>
@@ -6146,6 +6563,12 @@
       <c r="B350" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C350" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="D350" s="1" t="s">
+        <v>266</v>
+      </c>
       <c r="E350" s="1" t="s">
         <v>35</v>
       </c>
@@ -6230,6 +6653,12 @@
       <c r="B356" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C356" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D356" s="1" t="s">
+        <v>264</v>
+      </c>
       <c r="E356" s="1" t="s">
         <v>8</v>
       </c>
@@ -6307,17 +6736,23 @@
         <v>40</v>
       </c>
     </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A362" s="1" t="s">
+    <row r="362" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A362" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B362" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E362" s="1" t="s">
+      <c r="B362" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C362" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D362" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="E362" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F362" s="1">
+      <c r="F362" s="2">
         <v>31</v>
       </c>
     </row>
@@ -6398,6 +6833,12 @@
       <c r="B368" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C368" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D368" s="1" t="s">
+        <v>278</v>
+      </c>
       <c r="E368" s="1" t="s">
         <v>22</v>
       </c>
@@ -6454,6 +6895,9 @@
       <c r="B372" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C372" s="1" t="s">
+        <v>297</v>
+      </c>
       <c r="E372" s="1" t="s">
         <v>18</v>
       </c>
@@ -6524,6 +6968,12 @@
       <c r="B377" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C377" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D377" s="1" t="s">
+        <v>299</v>
+      </c>
       <c r="E377" s="1" t="s">
         <v>94</v>
       </c>
@@ -6591,6 +7041,9 @@
       <c r="B382" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C382" s="1" t="s">
+        <v>300</v>
+      </c>
       <c r="E382" s="1" t="s">
         <v>4</v>
       </c>
@@ -6633,6 +7086,12 @@
       <c r="B385" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C385" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="D385" s="1" t="s">
+        <v>302</v>
+      </c>
       <c r="E385" s="1" t="s">
         <v>14</v>
       </c>
@@ -6689,6 +7148,9 @@
       <c r="B389" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C389" s="1" t="s">
+        <v>303</v>
+      </c>
       <c r="E389" s="1" t="s">
         <v>21</v>
       </c>
@@ -6773,6 +7235,9 @@
       <c r="B395" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C395" s="1" t="s">
+        <v>304</v>
+      </c>
       <c r="E395" s="1" t="s">
         <v>24</v>
       </c>
@@ -6829,6 +7294,12 @@
       <c r="B399" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C399" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>306</v>
+      </c>
       <c r="E399" s="1" t="s">
         <v>84</v>
       </c>
@@ -6941,6 +7412,12 @@
       <c r="B407" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C407" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="E407" s="1" t="s">
         <v>49</v>
       </c>
@@ -6983,6 +7460,12 @@
       <c r="B410" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C410" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="D410" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="E410" s="1" t="s">
         <v>92</v>
       </c>
@@ -7011,6 +7494,9 @@
       <c r="B412" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C412" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="E412" s="1" t="s">
         <v>4</v>
       </c>
@@ -7081,6 +7567,9 @@
       <c r="B417" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C417" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="E417" s="1" t="s">
         <v>82</v>
       </c>
@@ -7165,6 +7654,12 @@
       <c r="B423" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C423" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="D423" s="1" t="s">
+        <v>306</v>
+      </c>
       <c r="E423" s="1" t="s">
         <v>84</v>
       </c>
@@ -7277,6 +7772,9 @@
       <c r="B431" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C431" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="E431" s="1" t="s">
         <v>23</v>
       </c>
@@ -7319,6 +7817,12 @@
       <c r="B434" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C434" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="D434" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="E434" s="1" t="s">
         <v>18</v>
       </c>
@@ -7389,6 +7893,12 @@
       <c r="B439" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C439" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D439" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="E439" s="1" t="s">
         <v>22</v>
       </c>
@@ -7459,6 +7969,12 @@
       <c r="B444" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C444" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="D444" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="E444" s="1" t="s">
         <v>23</v>
       </c>
@@ -7529,6 +8045,12 @@
       <c r="B449" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C449" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D449" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="E449" s="1" t="s">
         <v>40</v>
       </c>
@@ -7638,6 +8160,12 @@
       <c r="B457" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C457" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D457" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="E457" s="1" t="s">
         <v>49</v>
       </c>
@@ -7680,6 +8208,12 @@
       <c r="B460" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C460" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="D460" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="E460" s="1" t="s">
         <v>35</v>
       </c>
@@ -7708,6 +8242,9 @@
       <c r="B462" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C462" s="1" t="s">
+        <v>234</v>
+      </c>
       <c r="E462" s="1" t="s">
         <v>1</v>
       </c>
@@ -7792,6 +8329,9 @@
       <c r="B468" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C468" s="1" t="s">
+        <v>325</v>
+      </c>
       <c r="E468" s="1" t="s">
         <v>21</v>
       </c>
@@ -7862,6 +8402,12 @@
       <c r="B473" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C473" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="D473" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="E473" s="1" t="s">
         <v>60</v>
       </c>
@@ -7943,6 +8489,9 @@
       <c r="B479" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C479" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="E479" s="1" t="s">
         <v>21</v>
       </c>
@@ -8013,6 +8562,9 @@
       <c r="B484" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C484" s="1" t="s">
+        <v>329</v>
+      </c>
       <c r="E484" s="1" t="s">
         <v>58</v>
       </c>
@@ -8069,6 +8621,9 @@
       <c r="B488" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C488" s="1" t="s">
+        <v>196</v>
+      </c>
       <c r="E488" s="1" t="s">
         <v>4</v>
       </c>
@@ -8125,6 +8680,9 @@
       <c r="B492" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="C492" s="1" t="s">
+        <v>257</v>
+      </c>
       <c r="E492" s="1" t="s">
         <v>15</v>
       </c>
@@ -8153,6 +8711,12 @@
       <c r="B494" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C494" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="D494" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="E494" s="1" t="s">
         <v>51</v>
       </c>
@@ -8209,6 +8773,9 @@
       <c r="B498" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C498" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="E498" s="1" t="s">
         <v>108</v>
       </c>
@@ -8223,6 +8790,9 @@
       <c r="B499" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C499" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="E499" s="1" t="s">
         <v>58</v>
       </c>
@@ -8307,6 +8877,12 @@
       <c r="B505" s="1" t="s">
         <v>62</v>
       </c>
+      <c r="C505" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D505" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="E505" s="1" t="s">
         <v>93</v>
       </c>
@@ -19538,18 +20114,12 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F1307" xr:uid="{879570A1-7CB1-4100-A233-96AAAA92AA6B}"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E32 E80 E134 E557" xr:uid="{80326330-940A-462F-9090-B9ADB78C405C}">
+      <formula1>#REF!</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{80326330-940A-462F-9090-B9ADB78C405C}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E32 E80 E134 E557</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>